<commit_message>
implement new spark version
</commit_message>
<xml_diff>
--- a/flink/performance measures.xlsx
+++ b/flink/performance measures.xlsx
@@ -407,29 +407,29 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N9"/>
+  <dimension ref="A1:O9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="14" width="5.7109375" customWidth="1"/>
+    <col min="2" max="15" width="5.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -437,7 +437,7 @@
         <v>1</v>
       </c>
       <c r="C2" s="2">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="D2" s="2">
         <v>5</v>
@@ -445,11 +445,11 @@
       <c r="E2" s="2">
         <v>5</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="F2" s="2">
+        <v>5</v>
+      </c>
+      <c r="G2" s="2" t="s">
         <v>2</v>
-      </c>
-      <c r="G2" s="2">
-        <v>10</v>
       </c>
       <c r="H2" s="2">
         <v>10</v>
@@ -457,11 +457,11 @@
       <c r="I2" s="2">
         <v>10</v>
       </c>
-      <c r="J2" s="2" t="s">
+      <c r="J2" s="2">
+        <v>10</v>
+      </c>
+      <c r="K2" s="2" t="s">
         <v>3</v>
-      </c>
-      <c r="K2" s="2">
-        <v>20</v>
       </c>
       <c r="L2" s="2">
         <v>20</v>
@@ -469,81 +469,87 @@
       <c r="M2" s="2">
         <v>20</v>
       </c>
-      <c r="N2" s="2" t="s">
+      <c r="N2" s="2">
+        <v>20</v>
+      </c>
+      <c r="O2" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="3">
         <v>565.44799999999998</v>
       </c>
-      <c r="C3" s="2">
+      <c r="C3" s="3">
+        <v>523.58600000000001</v>
+      </c>
+      <c r="D3" s="2">
         <v>84.8</v>
       </c>
-      <c r="D3" s="2">
+      <c r="E3" s="2">
         <v>71.685000000000002</v>
       </c>
-      <c r="E3" s="2">
+      <c r="F3" s="2">
         <v>115.098</v>
       </c>
-      <c r="F3" s="2">
-        <f>SUM(C3:E3)/3</f>
+      <c r="G3" s="2">
+        <f>SUM(D3:F3)/3</f>
         <v>90.527666666666676</v>
       </c>
-      <c r="G3" s="2">
+      <c r="H3" s="2">
         <v>36.9</v>
       </c>
-      <c r="H3" s="2">
+      <c r="I3" s="2">
         <v>43.210999999999999</v>
       </c>
-      <c r="I3" s="2">
+      <c r="J3" s="2">
         <v>56.427999999999997</v>
       </c>
-      <c r="J3" s="2">
-        <f>SUM(G3:I3)/3</f>
+      <c r="K3" s="2">
+        <f>SUM(H3:J3)/3</f>
         <v>45.512999999999998</v>
       </c>
-      <c r="K3" s="2">
+      <c r="L3" s="2">
         <v>41.887999999999998</v>
       </c>
-      <c r="L3" s="2">
+      <c r="M3" s="2">
         <v>38.642000000000003</v>
       </c>
-      <c r="M3" s="2">
+      <c r="N3" s="2">
         <v>34.951999999999998</v>
       </c>
-      <c r="N3" s="2">
-        <f>SUM(K3:M3)/3</f>
+      <c r="O3" s="2">
+        <f>SUM(L3:N3)/3</f>
         <v>38.494</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>8</v>
       </c>
-      <c r="G4">
+      <c r="H4">
         <v>15.5</v>
       </c>
-      <c r="H4">
+      <c r="I4">
         <v>14</v>
       </c>
-      <c r="I4">
+      <c r="J4">
         <v>19.600000000000001</v>
       </c>
-      <c r="K4">
+      <c r="L4">
         <v>14.4</v>
       </c>
-      <c r="L4">
+      <c r="M4">
         <v>13.6</v>
       </c>
-      <c r="M4">
+      <c r="N4">
         <v>13.7</v>
       </c>
     </row>
-    <row r="9" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="9" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
add performance for newSpark
</commit_message>
<xml_diff>
--- a/flink/performance measures.xlsx
+++ b/flink/performance measures.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Performance" sheetId="1" r:id="rId1"/>
+    <sheet name="Spark" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="43">
   <si>
     <t>5 Durchschnitt</t>
   </si>
@@ -71,6 +72,78 @@
   </si>
   <si>
     <t>&gt;70min</t>
+  </si>
+  <si>
+    <t>ncvoter1k</t>
+  </si>
+  <si>
+    <t>ncvoter10k</t>
+  </si>
+  <si>
+    <t>table</t>
+  </si>
+  <si>
+    <t>rows</t>
+  </si>
+  <si>
+    <t>columns</t>
+  </si>
+  <si>
+    <t>iterations</t>
+  </si>
+  <si>
+    <t>candidates to check</t>
+  </si>
+  <si>
+    <t>iteration</t>
+  </si>
+  <si>
+    <t>candidates</t>
+  </si>
+  <si>
+    <t>isEmptyCheck</t>
+  </si>
+  <si>
+    <t>?</t>
+  </si>
+  <si>
+    <t>no unpersist</t>
+  </si>
+  <si>
+    <t>cache before unpersist</t>
+  </si>
+  <si>
+    <t>15c</t>
+  </si>
+  <si>
+    <t>nvoter20k</t>
+  </si>
+  <si>
+    <t>ncvoter20k</t>
+  </si>
+  <si>
+    <t>ncvoter30k</t>
+  </si>
+  <si>
+    <t>20k</t>
+  </si>
+  <si>
+    <t>30k</t>
+  </si>
+  <si>
+    <t>fd_reduced</t>
+  </si>
+  <si>
+    <t>fd reduced</t>
+  </si>
+  <si>
+    <t>time</t>
+  </si>
+  <si>
+    <t>&gt;12*60</t>
+  </si>
+  <si>
+    <t>etwa 2 h</t>
   </si>
 </sst>
 </file>
@@ -363,11 +436,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="105020800"/>
-        <c:axId val="105022592"/>
+        <c:axId val="159818496"/>
+        <c:axId val="159820032"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="105020800"/>
+        <c:axId val="159818496"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -377,7 +450,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="105022592"/>
+        <c:crossAx val="159820032"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -385,7 +458,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="105022592"/>
+        <c:axId val="159820032"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -396,7 +469,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="105020800"/>
+        <c:crossAx val="159818496"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -613,11 +686,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="105044224"/>
-        <c:axId val="105582592"/>
+        <c:axId val="160583040"/>
+        <c:axId val="160584832"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="105044224"/>
+        <c:axId val="160583040"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -627,7 +700,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="105582592"/>
+        <c:crossAx val="160584832"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -635,7 +708,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="105582592"/>
+        <c:axId val="160584832"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -646,14 +719,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="105044224"/>
+        <c:crossAx val="160583040"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1024,8 +1096,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="L32" sqref="L32"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17:E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1492,4 +1564,846 @@
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G75"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B1">
+        <v>20</v>
+      </c>
+      <c r="C1">
+        <v>15</v>
+      </c>
+      <c r="D1">
+        <v>10</v>
+      </c>
+      <c r="E1">
+        <v>5</v>
+      </c>
+      <c r="F1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" s="5">
+        <v>45</v>
+      </c>
+      <c r="C2" s="5">
+        <v>47.5</v>
+      </c>
+      <c r="D2" s="5">
+        <v>50</v>
+      </c>
+      <c r="E2" s="5">
+        <v>54</v>
+      </c>
+      <c r="F2" s="5">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3">
+        <v>266.5</v>
+      </c>
+      <c r="C3">
+        <v>329</v>
+      </c>
+      <c r="D3">
+        <v>348</v>
+      </c>
+      <c r="F3">
+        <v>1833</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>33</v>
+      </c>
+      <c r="B4">
+        <v>650</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>35</v>
+      </c>
+      <c r="B5">
+        <v>1349</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>38</v>
+      </c>
+      <c r="B6" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>21</v>
+      </c>
+      <c r="B12" t="s">
+        <v>22</v>
+      </c>
+      <c r="C12" t="s">
+        <v>23</v>
+      </c>
+      <c r="D12" t="s">
+        <v>24</v>
+      </c>
+      <c r="E12" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>19</v>
+      </c>
+      <c r="B13">
+        <v>1000</v>
+      </c>
+      <c r="C13">
+        <v>19</v>
+      </c>
+      <c r="D13">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>20</v>
+      </c>
+      <c r="B14">
+        <v>10000</v>
+      </c>
+      <c r="C14">
+        <v>19</v>
+      </c>
+      <c r="D14">
+        <v>17</v>
+      </c>
+      <c r="E14">
+        <v>166601</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>34</v>
+      </c>
+      <c r="B15">
+        <v>20000</v>
+      </c>
+      <c r="C15">
+        <v>19</v>
+      </c>
+      <c r="D15">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>35</v>
+      </c>
+      <c r="B16">
+        <v>30000</v>
+      </c>
+      <c r="C16">
+        <v>19</v>
+      </c>
+      <c r="D16">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>38</v>
+      </c>
+      <c r="B17">
+        <v>250000</v>
+      </c>
+      <c r="C17">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>21</v>
+      </c>
+      <c r="B22" t="s">
+        <v>26</v>
+      </c>
+      <c r="C22" t="s">
+        <v>27</v>
+      </c>
+      <c r="D22" t="s">
+        <v>28</v>
+      </c>
+      <c r="E22" t="s">
+        <v>31</v>
+      </c>
+      <c r="F22" t="s">
+        <v>30</v>
+      </c>
+      <c r="G22" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>20</v>
+      </c>
+      <c r="B23">
+        <v>1</v>
+      </c>
+      <c r="C23">
+        <v>19</v>
+      </c>
+      <c r="D23" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B24">
+        <v>2</v>
+      </c>
+      <c r="C24">
+        <v>171</v>
+      </c>
+      <c r="D24">
+        <v>4</v>
+      </c>
+      <c r="E24">
+        <v>0.1</v>
+      </c>
+      <c r="F24">
+        <v>0.2</v>
+      </c>
+      <c r="G24">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B25">
+        <v>3</v>
+      </c>
+      <c r="C25">
+        <v>969</v>
+      </c>
+      <c r="D25">
+        <v>4</v>
+      </c>
+      <c r="E25">
+        <v>3</v>
+      </c>
+      <c r="F25">
+        <v>3</v>
+      </c>
+      <c r="G25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B26">
+        <v>4</v>
+      </c>
+      <c r="C26">
+        <v>3512</v>
+      </c>
+      <c r="D26">
+        <v>3</v>
+      </c>
+      <c r="E26">
+        <v>3</v>
+      </c>
+      <c r="F26">
+        <v>3</v>
+      </c>
+      <c r="G26">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B27">
+        <v>5</v>
+      </c>
+      <c r="C27">
+        <v>9087</v>
+      </c>
+      <c r="D27">
+        <v>3</v>
+      </c>
+      <c r="E27">
+        <v>2</v>
+      </c>
+      <c r="F27">
+        <v>3</v>
+      </c>
+      <c r="G27">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B28">
+        <v>6</v>
+      </c>
+      <c r="C28">
+        <v>17685</v>
+      </c>
+      <c r="D28">
+        <v>5</v>
+      </c>
+      <c r="E28">
+        <v>4</v>
+      </c>
+      <c r="F28">
+        <v>5</v>
+      </c>
+      <c r="G28">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B29">
+        <v>7</v>
+      </c>
+      <c r="C29">
+        <v>26591</v>
+      </c>
+      <c r="D29">
+        <v>12</v>
+      </c>
+      <c r="E29">
+        <v>12</v>
+      </c>
+      <c r="F29">
+        <v>10</v>
+      </c>
+      <c r="G29">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B30">
+        <v>8</v>
+      </c>
+      <c r="C30">
+        <v>31601</v>
+      </c>
+      <c r="D30">
+        <v>23</v>
+      </c>
+      <c r="E30">
+        <v>22</v>
+      </c>
+      <c r="F30">
+        <v>19</v>
+      </c>
+      <c r="G30">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B31">
+        <v>9</v>
+      </c>
+      <c r="C31">
+        <v>30045</v>
+      </c>
+      <c r="D31">
+        <v>42</v>
+      </c>
+      <c r="E31">
+        <v>39</v>
+      </c>
+      <c r="F31">
+        <v>31</v>
+      </c>
+      <c r="G31">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B32">
+        <v>10</v>
+      </c>
+      <c r="C32">
+        <v>22913</v>
+      </c>
+      <c r="D32">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="E32">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="F32">
+        <v>41</v>
+      </c>
+      <c r="G32">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B33">
+        <v>11</v>
+      </c>
+      <c r="C33">
+        <v>13952</v>
+      </c>
+      <c r="D33">
+        <v>1.4</v>
+      </c>
+      <c r="E33">
+        <v>1.5</v>
+      </c>
+      <c r="F33">
+        <v>41</v>
+      </c>
+      <c r="G33">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B34">
+        <v>12</v>
+      </c>
+      <c r="C34">
+        <v>6708</v>
+      </c>
+      <c r="D34">
+        <v>1.7</v>
+      </c>
+      <c r="E34">
+        <v>1.7</v>
+      </c>
+      <c r="F34">
+        <v>36</v>
+      </c>
+      <c r="G34">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B35">
+        <v>13</v>
+      </c>
+      <c r="C35">
+        <v>2497</v>
+      </c>
+      <c r="D35">
+        <v>1.8</v>
+      </c>
+      <c r="F35">
+        <v>26</v>
+      </c>
+      <c r="G35">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B36">
+        <v>14</v>
+      </c>
+      <c r="C36">
+        <v>696</v>
+      </c>
+      <c r="D36">
+        <v>1.9</v>
+      </c>
+      <c r="F36">
+        <v>13</v>
+      </c>
+      <c r="G36">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B37">
+        <v>15</v>
+      </c>
+      <c r="C37">
+        <v>137</v>
+      </c>
+      <c r="D37">
+        <v>1.9</v>
+      </c>
+      <c r="F37">
+        <v>6</v>
+      </c>
+      <c r="G37">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B38">
+        <v>16</v>
+      </c>
+      <c r="C38">
+        <v>17</v>
+      </c>
+      <c r="D38">
+        <v>1.9</v>
+      </c>
+      <c r="F38">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B39">
+        <v>17</v>
+      </c>
+      <c r="C39">
+        <v>1</v>
+      </c>
+      <c r="D39">
+        <v>1.9</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D41" t="s">
+        <v>36</v>
+      </c>
+      <c r="F41" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>34</v>
+      </c>
+      <c r="B42">
+        <v>1</v>
+      </c>
+      <c r="C42">
+        <v>19</v>
+      </c>
+      <c r="E42">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B43">
+        <v>2</v>
+      </c>
+      <c r="D43">
+        <v>1</v>
+      </c>
+      <c r="F43">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B44">
+        <v>3</v>
+      </c>
+      <c r="D44">
+        <v>2</v>
+      </c>
+      <c r="F44">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B45">
+        <v>4</v>
+      </c>
+      <c r="D45">
+        <v>3</v>
+      </c>
+      <c r="F45">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B46">
+        <v>5</v>
+      </c>
+      <c r="D46">
+        <v>4</v>
+      </c>
+      <c r="F46">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B47">
+        <v>6</v>
+      </c>
+      <c r="D47">
+        <v>9</v>
+      </c>
+      <c r="F47">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B48">
+        <v>7</v>
+      </c>
+      <c r="D48">
+        <v>23</v>
+      </c>
+      <c r="F48">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B49">
+        <v>8</v>
+      </c>
+      <c r="D49">
+        <v>51</v>
+      </c>
+      <c r="F49">
+        <f>1.6*60</f>
+        <v>96</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B50">
+        <v>9</v>
+      </c>
+      <c r="D50">
+        <f>1.4*60</f>
+        <v>84</v>
+      </c>
+      <c r="F50">
+        <f>2.7*60</f>
+        <v>162</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B51">
+        <v>10</v>
+      </c>
+      <c r="D51">
+        <f>1.9*60</f>
+        <v>114</v>
+      </c>
+      <c r="F51">
+        <f>3.8 * 60</f>
+        <v>228</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B52">
+        <v>11</v>
+      </c>
+      <c r="D52">
+        <f>1.9*60</f>
+        <v>114</v>
+      </c>
+      <c r="F52">
+        <f>4.2*60</f>
+        <v>252</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B53">
+        <v>12</v>
+      </c>
+      <c r="D53">
+        <f>1.6*60</f>
+        <v>96</v>
+      </c>
+      <c r="F53">
+        <f>3.6*60</f>
+        <v>216</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B54">
+        <v>13</v>
+      </c>
+      <c r="F54">
+        <f>2.5*60</f>
+        <v>150</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B55">
+        <v>14</v>
+      </c>
+      <c r="F55">
+        <f>1.4*60</f>
+        <v>84</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B56">
+        <v>15</v>
+      </c>
+      <c r="F56">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B57">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B58">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>39</v>
+      </c>
+      <c r="B60" t="s">
+        <v>26</v>
+      </c>
+      <c r="C60" t="s">
+        <v>40</v>
+      </c>
+      <c r="D60" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B61">
+        <v>1</v>
+      </c>
+      <c r="D61">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B62">
+        <v>2</v>
+      </c>
+      <c r="C62">
+        <v>1</v>
+      </c>
+      <c r="D62">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B63">
+        <v>3</v>
+      </c>
+      <c r="C63">
+        <v>7</v>
+      </c>
+      <c r="D63">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B64">
+        <v>4</v>
+      </c>
+      <c r="C64">
+        <v>19</v>
+      </c>
+      <c r="D64">
+        <v>1365</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B65">
+        <v>5</v>
+      </c>
+      <c r="C65">
+        <v>50</v>
+      </c>
+      <c r="D65">
+        <v>3003</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B66">
+        <v>6</v>
+      </c>
+      <c r="C66">
+        <f>2.8*60</f>
+        <v>168</v>
+      </c>
+      <c r="D66">
+        <v>5005</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B67">
+        <v>7</v>
+      </c>
+      <c r="C67">
+        <f>5.9*60</f>
+        <v>354</v>
+      </c>
+      <c r="D67">
+        <v>6435</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B68">
+        <v>8</v>
+      </c>
+      <c r="C68">
+        <f>14*60</f>
+        <v>840</v>
+      </c>
+      <c r="D68">
+        <v>6435</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B69">
+        <v>9</v>
+      </c>
+      <c r="C69" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B70">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B71">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B72">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B73">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B74">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A75">
+        <f>1439/60</f>
+        <v>23.983333333333334</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>